<commit_message>
Version Final del Test Case
</commit_message>
<xml_diff>
--- a/Temp/Medallero_Olimpico.xlsx
+++ b/Temp/Medallero_Olimpico.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\070804781\Documents\UiPath\TASK_Case_Roboyo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{414C9C69-1D47-47D7-B5F1-EB5A206F8E1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E60CC9B-E417-47ED-9D8A-2C51CDB5936B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="855" yWindow="855" windowWidth="19920" windowHeight="10440" activeTab="2" xr2:uid="{BA963F06-9B00-4F5A-A984-3F67E39AA76D}"/>
+    <workbookView xWindow="855" yWindow="855" windowWidth="19920" windowHeight="10440" activeTab="2" xr2:uid="{214FAD7F-17BC-428B-A94E-167DE9AA2566}"/>
   </bookViews>
   <sheets>
     <sheet name="Oro" sheetId="1" r:id="rId1"/>
@@ -591,7 +591,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05EC9D31-6B8C-49CA-8B1B-C384A4131A09}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABBBC955-B113-45A8-9C77-6E452FC51E35}">
   <dimension ref="A1:D60"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1267,7 +1267,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D724BE8-15B9-443E-9B93-E346B6E494D5}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABBF2674-F4E8-422E-9AAC-300213D3AC69}">
   <dimension ref="A1:D60"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1943,7 +1943,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFF37E48-4147-4B91-82F7-0FBD023E9E8E}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC635BCF-6557-4B72-8805-89CBFECFA929}">
   <dimension ref="A1:D60"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>